<commit_message>
Solucion del bug de pago billete a billete
</commit_message>
<xml_diff>
--- a/resource/output_example.xlsx
+++ b/resource/output_example.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="392" documentId="11_6F474AE45A59140F62355476585DCE3A87CEE3AB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6FC6F38-E21A-4AB3-8DAE-61DEC6FF106E}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19905" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ventas" sheetId="1" r:id="rId1"/>
@@ -572,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -598,10 +598,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -610,16 +619,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2273,7 +2272,7 @@
       <c r="E1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="17" t="s">
         <v>61</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -2303,7 +2302,7 @@
       <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="17" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2317,7 +2316,7 @@
       <c r="C2" s="16">
         <v>2</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="18">
         <v>6035</v>
       </c>
       <c r="E2" s="16" t="s">
@@ -2358,7 +2357,7 @@
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
-      <c r="D3" s="23"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="16" t="s">
         <v>8</v>
       </c>
@@ -2393,7 +2392,7 @@
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
-      <c r="D4" s="23"/>
+      <c r="D4" s="18"/>
       <c r="E4" s="16" t="s">
         <v>67</v>
       </c>
@@ -2428,7 +2427,7 @@
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
-      <c r="D5" s="23"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="16" t="s">
         <v>68</v>
       </c>
@@ -2463,7 +2462,7 @@
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
-      <c r="D6" s="23"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="16" t="s">
         <v>69</v>
       </c>
@@ -2498,7 +2497,7 @@
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
-      <c r="D7" s="23"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="16" t="s">
         <v>70</v>
       </c>
@@ -2533,7 +2532,7 @@
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
-      <c r="D8" s="23"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="16" t="s">
         <v>5</v>
       </c>
@@ -2580,7 +2579,7 @@
       <c r="E9" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="9">
         <v>146361</v>
       </c>
       <c r="G9" s="16">
@@ -3743,48 +3742,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="21"/>
+      <c r="D1" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="21"/>
+      <c r="G1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="J1" s="19" t="s">
+      <c r="H1" s="21"/>
+      <c r="J1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="M1" s="19" t="s">
+      <c r="K1" s="23"/>
+      <c r="M1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="P1" s="19" t="s">
+      <c r="N1" s="23"/>
+      <c r="P1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="20"/>
-      <c r="S1" s="19" t="s">
+      <c r="Q1" s="23"/>
+      <c r="S1" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="20"/>
+      <c r="T1" s="23"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="D2" s="21" t="s">
+      <c r="B2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="G2" s="21" t="s">
+      <c r="E2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="19"/>
       <c r="J2" s="5" t="s">
         <v>47</v>
       </c>
@@ -4079,18 +4078,18 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="D8" s="18" t="s">
+      <c r="B8" s="20"/>
+      <c r="D8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="G8" s="18" t="s">
+      <c r="E8" s="20"/>
+      <c r="G8" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="18"/>
+      <c r="H8" s="20"/>
       <c r="J8" s="5" t="s">
         <v>30</v>
       </c>
@@ -4319,18 +4318,18 @@
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="D15" s="18" t="s">
+      <c r="B15" s="20"/>
+      <c r="D15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="G15" s="18" t="s">
+      <c r="E15" s="20"/>
+      <c r="G15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="18"/>
+      <c r="H15" s="20"/>
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -4453,18 +4452,18 @@
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="D22" s="21" t="s">
+      <c r="B22" s="19"/>
+      <c r="D22" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="G22" s="21" t="s">
+      <c r="E22" s="19"/>
+      <c r="G22" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="21"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:58" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -4649,18 +4648,18 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="D29" s="21" t="s">
+      <c r="B29" s="19"/>
+      <c r="D29" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="21"/>
-      <c r="G29" s="21" t="s">
+      <c r="E29" s="19"/>
+      <c r="G29" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H29" s="21"/>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -4727,18 +4726,18 @@
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="D34" s="21" t="s">
+      <c r="B34" s="19"/>
+      <c r="D34" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="21"/>
-      <c r="G34" s="21" t="s">
+      <c r="E34" s="19"/>
+      <c r="G34" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="21"/>
+      <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -4771,18 +4770,18 @@
       <c r="B36" s="6"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="D37" s="21" t="s">
+      <c r="B37" s="19"/>
+      <c r="D37" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="G37" s="21" t="s">
+      <c r="E37" s="19"/>
+      <c r="G37" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H37" s="21"/>
+      <c r="H37" s="19"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -4812,6 +4811,23 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="D37:E37"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A2:B2"/>
@@ -4823,23 +4839,6 @@
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>